<commit_message>
Final version pre paper
</commit_message>
<xml_diff>
--- a/ORDER.xlsx
+++ b/ORDER.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="22">
   <si>
     <t>protocol</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>frontal patient #4: did vis first</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>vb</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>pb</t>
+  </si>
+  <si>
+    <t>not going to use her</t>
+  </si>
+  <si>
+    <t>whree we stoped the first time</t>
   </si>
 </sst>
 </file>
@@ -105,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -179,11 +197,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -211,6 +262,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,20 +566,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:16">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:16">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -541,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:16">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -561,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:16">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -581,7 +637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:16">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -601,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:16">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -621,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:16">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -641,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:16">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -661,7 +717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:16">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -681,7 +737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:16">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -701,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:16">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -721,7 +777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:16">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -741,7 +797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:16">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -761,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:16">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -781,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:16">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -800,8 +856,20 @@
       <c r="F16" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="M16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -820,8 +888,20 @@
       <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="M17" s="6">
+        <v>2</v>
+      </c>
+      <c r="N17" s="6">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -840,8 +920,20 @@
       <c r="F18" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="M18" s="6">
+        <v>6</v>
+      </c>
+      <c r="N18" s="6">
+        <v>7</v>
+      </c>
+      <c r="O18" s="6">
+        <v>4</v>
+      </c>
+      <c r="P18" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="6">
         <v>16</v>
       </c>
@@ -863,8 +955,20 @@
       <c r="I19" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="M19" s="6">
+        <v>10</v>
+      </c>
+      <c r="N19" s="6">
+        <v>11</v>
+      </c>
+      <c r="O19" s="6">
+        <v>8</v>
+      </c>
+      <c r="P19" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="6">
         <v>17</v>
       </c>
@@ -886,8 +990,20 @@
       <c r="I20" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="M20" s="6">
+        <v>14</v>
+      </c>
+      <c r="N20" s="6">
+        <v>15</v>
+      </c>
+      <c r="O20" s="6">
+        <v>12</v>
+      </c>
+      <c r="P20" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="6">
         <v>18</v>
       </c>
@@ -906,8 +1022,20 @@
       <c r="F21" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="M21" s="6">
+        <v>18</v>
+      </c>
+      <c r="N21" s="6">
+        <v>19</v>
+      </c>
+      <c r="O21" s="6">
+        <v>16</v>
+      </c>
+      <c r="P21" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="6">
         <v>19</v>
       </c>
@@ -926,8 +1054,20 @@
       <c r="F22" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="M22" s="23">
+        <v>20</v>
+      </c>
+      <c r="N22" s="11">
+        <v>22</v>
+      </c>
+      <c r="O22" s="16">
+        <v>32</v>
+      </c>
+      <c r="P22" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="23">
         <v>20</v>
       </c>
@@ -949,8 +1089,20 @@
       <c r="G23" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="M23" s="11">
+        <v>21</v>
+      </c>
+      <c r="N23" s="16">
+        <v>30</v>
+      </c>
+      <c r="O23" s="6">
+        <v>37</v>
+      </c>
+      <c r="P23" s="6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="11">
         <v>21</v>
       </c>
@@ -972,8 +1124,20 @@
       <c r="G24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="M24" s="16">
+        <v>27</v>
+      </c>
+      <c r="N24" s="6">
+        <v>36</v>
+      </c>
+      <c r="O24" s="6">
+        <v>41</v>
+      </c>
+      <c r="P24" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="11">
         <v>22</v>
       </c>
@@ -995,8 +1159,20 @@
       <c r="G25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="M25" s="6">
+        <v>35</v>
+      </c>
+      <c r="N25" s="6">
+        <v>40</v>
+      </c>
+      <c r="O25" s="6">
+        <v>45</v>
+      </c>
+      <c r="P25" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="16">
         <v>27</v>
       </c>
@@ -1015,8 +1191,20 @@
       <c r="F26" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="M26" s="6">
+        <v>39</v>
+      </c>
+      <c r="N26" s="6">
+        <v>44</v>
+      </c>
+      <c r="O26" s="6">
+        <v>49</v>
+      </c>
+      <c r="P26" s="27">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="16">
         <v>30</v>
       </c>
@@ -1035,8 +1223,17 @@
       <c r="F27" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="M27" s="6">
+        <v>43</v>
+      </c>
+      <c r="N27" s="6">
+        <v>48</v>
+      </c>
+      <c r="O27" s="27">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="16">
         <v>32</v>
       </c>
@@ -1055,8 +1252,11 @@
       <c r="F28" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="M28" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="16">
         <v>34</v>
       </c>
@@ -1076,7 +1276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:16">
       <c r="A30" s="6">
         <v>35</v>
       </c>
@@ -1096,7 +1296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:16">
       <c r="A31" s="6">
         <v>36</v>
       </c>
@@ -1115,8 +1315,20 @@
       <c r="F31" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="M31">
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <v>11</v>
+      </c>
+      <c r="O31">
+        <v>10</v>
+      </c>
+      <c r="P31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="6">
         <v>37</v>
       </c>
@@ -1135,8 +1347,14 @@
       <c r="F32" s="26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="N32">
+        <v>23</v>
+      </c>
+      <c r="P32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="6">
         <v>38</v>
       </c>
@@ -1156,7 +1374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" s="6">
         <v>39</v>
       </c>
@@ -1176,7 +1394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7">
       <c r="A35" s="6">
         <v>40</v>
       </c>
@@ -1196,7 +1414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7">
       <c r="A36" s="6">
         <v>41</v>
       </c>
@@ -1216,7 +1434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7">
       <c r="A37" s="6">
         <v>42</v>
       </c>
@@ -1236,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="A38" s="6">
         <v>43</v>
       </c>
@@ -1256,7 +1474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7">
       <c r="A39" s="6">
         <v>44</v>
       </c>
@@ -1272,8 +1490,11 @@
       <c r="E39" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="F39" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="6">
         <v>45</v>
       </c>
@@ -1289,8 +1510,11 @@
       <c r="E40" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="F40" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="6">
         <v>46</v>
       </c>
@@ -1306,8 +1530,11 @@
       <c r="E41" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="F41" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="6">
         <v>47</v>
       </c>
@@ -1323,8 +1550,11 @@
       <c r="E42" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="F42" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="6">
         <v>48</v>
       </c>
@@ -1340,8 +1570,11 @@
       <c r="E43" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="F43" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="6">
         <v>49</v>
       </c>
@@ -1357,8 +1590,11 @@
       <c r="E44" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="6">
         <v>50</v>
       </c>
@@ -1372,6 +1608,165 @@
         <v>5</v>
       </c>
       <c r="E45" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="6">
+        <v>51</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="30">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="6">
+        <v>54</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="27">
+        <v>53</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="B50" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="B51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="B52" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="B54" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>